<commit_message>
removed config json from the code
</commit_message>
<xml_diff>
--- a/Week02_report.xlsx
+++ b/Week02_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="62">
   <si>
     <t>Student ID</t>
   </si>
@@ -190,9 +190,6 @@
     <t>download_figma_and_install</t>
   </si>
   <si>
-    <t>create_canva-menu</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -202,7 +199,7 @@
     <t>Week: Week02</t>
   </si>
   <si>
-    <t>Generated: 2023-09-02 11:44:08 AM</t>
+    <t>Generated: 2023-09-02 12:00:19 PM</t>
   </si>
 </sst>
 </file>
@@ -614,7 +611,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -631,7 +628,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -645,7 +642,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -659,7 +656,7 @@
         <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -676,7 +673,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -693,7 +690,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -710,7 +707,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -727,7 +724,7 @@
         <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -741,7 +738,7 @@
         <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -758,7 +755,7 @@
         <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -775,7 +772,7 @@
         <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -792,7 +789,7 @@
         <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -809,7 +806,7 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -826,7 +823,7 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -843,7 +840,7 @@
         <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -860,7 +857,7 @@
         <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -877,7 +874,7 @@
         <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -894,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -911,7 +908,7 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -925,7 +922,7 @@
         <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -939,7 +936,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -956,7 +953,7 @@
         <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -973,7 +970,7 @@
         <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -990,34 +987,31 @@
         <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 2 tasks added
</commit_message>
<xml_diff>
--- a/Week02_report.xlsx
+++ b/Week02_report.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SwathipriyaSundaram\Students report\StudentsReport\StudentsReport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B21839B-E669-436C-994D-7384DEEDEBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
   <si>
     <t>Student ID</t>
   </si>
@@ -217,8 +223,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,13 +300,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +352,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -372,6 +386,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -406,9 +421,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -581,12 +597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
@@ -596,7 +614,7 @@
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -633,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -653,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -670,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -687,7 +705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -704,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -724,7 +742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -744,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -761,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -778,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -795,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -812,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -832,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -852,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -872,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -892,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -912,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -932,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -952,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -972,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -992,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1009,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1026,27 +1044,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>58</v>
       </c>
-      <c r="D24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" t="s">
-        <v>63</v>
+      <c r="E24" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1063,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1100,12 +1115,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>

</xml_diff>